<commit_message>
adding permutation with word
</commit_message>
<xml_diff>
--- a/resources/combinatorics.xlsx
+++ b/resources/combinatorics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proiecte\CombinatoricsTools\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbabiuc\CLionProjects\CombinatoricsTools\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E414B2-8DD5-42E1-892F-AF55FAA2B068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDC5B9A-E602-44F0-BEDE-A500F556A83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,39 +196,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -243,8 +219,33 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -528,35 +529,35 @@
   <dimension ref="E3:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="I3" s="6" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="12"/>
+      <c r="I3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="N3" s="6" t="s">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="N3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="S3" s="6" t="s">
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="S3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
     </row>
     <row r="4" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E4" s="1">
@@ -568,7 +569,7 @@
       <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -580,7 +581,7 @@
       <c r="L4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -592,7 +593,7 @@
       <c r="Q4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="T4" s="1" t="s">
@@ -625,10 +626,10 @@
         <v>3</v>
       </c>
       <c r="K5" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N5" s="1">
         <v>6</v>
@@ -656,65 +657,65 @@
       </c>
     </row>
     <row r="6" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="I6" s="2">
+      <c r="I6" s="11">
         <f>(FACT(I5))/(FACT(J5)*FACT(I5-J5))</f>
         <v>35</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="2">
+      <c r="J6" s="12"/>
+      <c r="K6" s="11">
         <f>(FACT(K5))/(FACT(L5)*FACT(K5-L5))</f>
-        <v>70</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="N6" s="2">
+        <v>210</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="N6" s="11">
         <f>(FACT(N5))/(FACT(N5-O5))</f>
         <v>120</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="2">
+      <c r="O6" s="12"/>
+      <c r="P6" s="11">
         <f>(FACT(P5))/(FACT(P5-Q5))</f>
         <v>56</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="S6" s="8">
+      <c r="Q6" s="12"/>
+      <c r="S6" s="3">
         <f>FACT(S5)</f>
         <v>5040</v>
       </c>
-      <c r="T6" s="8">
+      <c r="T6" s="3">
         <f t="shared" ref="T6:V6" si="1">FACT(T5)</f>
         <v>6</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="3">
         <f t="shared" si="1"/>
         <v>40320</v>
       </c>
-      <c r="V6" s="8">
+      <c r="V6" s="18">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="N9" s="6" t="s">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="N9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="S9" s="6" t="s">
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="S9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
     </row>
     <row r="10" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -726,7 +727,7 @@
       <c r="L10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -738,14 +739,14 @@
       <c r="Q10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
+      <c r="S10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
     </row>
     <row r="11" spans="5:22" x14ac:dyDescent="0.25">
       <c r="I11" s="1">
@@ -786,109 +787,109 @@
       </c>
     </row>
     <row r="12" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="I12" s="2">
+      <c r="I12" s="11">
         <f>(FACT(J11+I11-1))/(FACT(I11-1)*FACT(J11))</f>
         <v>35</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="2">
+      <c r="J12" s="12"/>
+      <c r="K12" s="11">
         <f>(FACT(L11+K11-1))/(FACT(K11-1)*FACT(L11))</f>
         <v>84</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="N12" s="2">
+      <c r="L12" s="12"/>
+      <c r="N12" s="11">
         <f>N11^O11</f>
         <v>216</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="2">
+      <c r="O12" s="12"/>
+      <c r="P12" s="11">
         <f>P11^Q11</f>
         <v>64</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="S12" s="6">
+      <c r="Q12" s="12"/>
+      <c r="S12" s="13">
         <f>FACT(SUM(T11:V11))/(FACT(T11)*FACT(U11)*FACT(V11))</f>
         <v>60</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
     </row>
     <row r="15" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="M16" s="5" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="M16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
     </row>
     <row r="17" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="13"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="5"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
     </row>
     <row r="19" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="14"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="F19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="6"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F20" s="1">
@@ -897,34 +898,34 @@
       <c r="G20" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="12">
-        <v>2</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
+      <c r="H20" s="4">
+        <v>2</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F21" s="2">
+      <c r="F21" s="11">
         <f>FACT(SUM(G20:H20))/(FACT(G20)*FACT(H20))</f>
         <v>6</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="13"/>
-      <c r="M21" s="6" t="s">
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="5"/>
+      <c r="M21" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="6"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="M22" s="7" t="s">
+      <c r="M22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N22" s="1" t="s">
@@ -932,7 +933,7 @@
       </c>
     </row>
     <row r="23" spans="6:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="8" t="s">
         <v>11</v>
       </c>
       <c r="M23" s="1">
@@ -943,37 +944,54 @@
       </c>
     </row>
     <row r="24" spans="6:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="11">
         <f>(FACT(M23))/(FACT(M23-N23))</f>
         <v>720</v>
       </c>
-      <c r="N24" s="4"/>
+      <c r="N24" s="12"/>
     </row>
     <row r="25" spans="6:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="6:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="6:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="6:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="8" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="S9:V9"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="S12:V12"/>
     <mergeCell ref="M16:T16"/>
     <mergeCell ref="M17:T20"/>
     <mergeCell ref="M24:N24"/>
@@ -983,23 +1001,6 @@
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="S9:V9"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>